<commit_message>
Done all the coding for my Chemistry IA, I could probably add MonteCarloMeasurements, but that's for another day.
</commit_message>
<xml_diff>
--- a/Excel Projects/Esterification Lab Data Logging.xlsx
+++ b/Excel Projects/Esterification Lab Data Logging.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wille\Desktop\Legacy-Projects-And-Code-Will-Martin\Excel Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19F3FA4-9AE4-4D46-8217-C1241D30A270}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB920CF-1AC7-4612-836A-F5AD6BA44E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2898" yWindow="2004" windowWidth="17280" windowHeight="8994" xr2:uid="{27043B7B-2271-401B-B46D-49CA3CF67942}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{27043B7B-2271-401B-B46D-49CA3CF67942}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="71">
   <si>
     <t>Trial 1 (30*C)</t>
   </si>
@@ -197,9 +197,6 @@
     <t>blank titration</t>
   </si>
   <si>
-    <t>base titration</t>
-  </si>
-  <si>
     <t>and this one, I didn't get the exact volume and they were over-titrated</t>
   </si>
   <si>
@@ -209,9 +206,6 @@
     <t>Started Reading Temperature ~30 seconds late</t>
   </si>
   <si>
-    <t>Note for 600 and onward, a 6-8g ice cube was added</t>
-  </si>
-  <si>
     <t>Trial 4 (30*C)</t>
   </si>
   <si>
@@ -252,6 +246,9 @@
   </si>
   <si>
     <t>edited?</t>
+  </si>
+  <si>
+    <t>±</t>
   </si>
 </sst>
 </file>
@@ -1063,347 +1060,6 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$Y$66</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Mol of Acetic Acid </c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$X$67:$X$74</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>45</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>180</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>360</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>600</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>720</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>900</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1080</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1260</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$Y$67:$Y$74</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>9.7249999999999993E-3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8.0749999999999971E-3</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.7750000000000006E-3</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.0250000000000008E-3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.1249999999999993E-3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.1250000000000011E-3</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4.7249999999999992E-3</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>4.9250000000000014E-3</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-AC83-4896-B216-DFAE20161ACE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="117213727"/>
-        <c:axId val="117221407"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="117213727"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="117221407"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="117221407"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="117213727"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
               <c:f>Sheet1!$Y$82</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
@@ -1696,7 +1352,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2221,46 +1877,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3810,522 +3426,6 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4881,16 +3981,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>3810</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>5715</xdr:rowOff>
+      <xdr:rowOff>1905</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>110490</xdr:colOff>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>5715</xdr:rowOff>
+      <xdr:rowOff>1905</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4910,42 +4010,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>3810</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>177165</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>37</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>79</xdr:row>
-      <xdr:rowOff>177165</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6EA8BC0E-9487-41A7-4166-4AA827F39589}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -4981,7 +4045,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5017,7 +4081,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5345,8 +4409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E9B97C-057F-4C1E-9083-78A721E3BFF1}">
   <dimension ref="B3:AD110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O47" workbookViewId="0">
-      <selection activeCell="P105" sqref="P105"/>
+    <sheetView tabSelected="1" topLeftCell="K47" workbookViewId="0">
+      <selection activeCell="Z51" sqref="Z51:Z59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5376,19 +4440,19 @@
         <v>2</v>
       </c>
       <c r="M3" t="s">
+        <v>55</v>
+      </c>
+      <c r="U3" t="s">
+        <v>57</v>
+      </c>
+      <c r="V3" t="s">
         <v>56</v>
       </c>
-      <c r="U3" t="s">
-        <v>59</v>
-      </c>
-      <c r="V3" t="s">
-        <v>58</v>
-      </c>
       <c r="AA3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="AB3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="2:30" x14ac:dyDescent="0.55000000000000004">
@@ -5508,7 +4572,7 @@
         <v>6.2999999999999989</v>
       </c>
       <c r="AD6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="2:30" x14ac:dyDescent="0.55000000000000004">
@@ -5534,7 +4598,7 @@
         <v>12.65</v>
       </c>
       <c r="L7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="U7" s="2">
         <v>0.54166666666666663</v>
@@ -5553,7 +4617,7 @@
         <v>5.7000000000000028</v>
       </c>
       <c r="AD7" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="2:30" x14ac:dyDescent="0.55000000000000004">
@@ -5601,7 +4665,7 @@
         <v>5.3999999999999986</v>
       </c>
       <c r="AD8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="2:30" x14ac:dyDescent="0.55000000000000004">
@@ -5630,7 +4694,7 @@
         <v>23.75</v>
       </c>
       <c r="M9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="U9" s="2">
         <v>0.875</v>
@@ -5639,7 +4703,7 @@
         <v>29.2</v>
       </c>
       <c r="W9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AA9" s="4">
         <v>1600</v>
@@ -5701,7 +4765,7 @@
         <v>4.8999999999999986</v>
       </c>
       <c r="AD10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="2:30" x14ac:dyDescent="0.55000000000000004">
@@ -5792,7 +4856,7 @@
         <v>30</v>
       </c>
       <c r="U13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="V13">
         <v>0.5</v>
@@ -6251,7 +5315,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="12:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="12:26" x14ac:dyDescent="0.55000000000000004">
       <c r="L49">
         <v>32</v>
       </c>
@@ -6259,7 +5323,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="50" spans="12:25" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="12:26" x14ac:dyDescent="0.55000000000000004">
       <c r="M50" t="s">
         <v>43</v>
       </c>
@@ -6284,8 +5348,11 @@
       <c r="Y50" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="12:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Z50" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="12:26" x14ac:dyDescent="0.55000000000000004">
       <c r="L51">
         <v>8.1</v>
       </c>
@@ -6323,8 +5390,12 @@
         <f t="shared" ref="Y51:Y59" si="5">S51*$V$51</f>
         <v>7.8750000000000001E-3</v>
       </c>
-    </row>
-    <row r="52" spans="12:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Z51">
+        <f>Y51*((0.05/N$51) + (0.05/M51))</f>
+        <v>9.2361111111111116E-4</v>
+      </c>
+    </row>
+    <row r="52" spans="12:26" x14ac:dyDescent="0.55000000000000004">
       <c r="L52">
         <v>15.9</v>
       </c>
@@ -6355,8 +5426,12 @@
         <f t="shared" si="5"/>
         <v>7.575000000000001E-3</v>
       </c>
-    </row>
-    <row r="53" spans="12:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Z52">
+        <f t="shared" ref="Z52:Z58" si="9">Y52*((0.05/N$51) + (0.05/M52))</f>
+        <v>8.9022435897435914E-4</v>
+      </c>
+    </row>
+    <row r="53" spans="12:26" x14ac:dyDescent="0.55000000000000004">
       <c r="L53">
         <v>23.3</v>
       </c>
@@ -6387,13 +5462,17 @@
         <f t="shared" si="5"/>
         <v>7.1750000000000008E-3</v>
       </c>
-    </row>
-    <row r="54" spans="12:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Z53">
+        <f t="shared" si="9"/>
+        <v>8.4570195195195208E-4</v>
+      </c>
+    </row>
+    <row r="54" spans="12:26" x14ac:dyDescent="0.55000000000000004">
       <c r="L54">
         <v>30.2</v>
       </c>
       <c r="M54">
-        <f t="shared" ref="M54:M56" si="9">L54-L53</f>
+        <f t="shared" ref="M54:M56" si="10">L54-L53</f>
         <v>6.8999999999999986</v>
       </c>
       <c r="O54">
@@ -6419,13 +5498,17 @@
         <f t="shared" si="5"/>
         <v>6.6749999999999986E-3</v>
       </c>
-    </row>
-    <row r="55" spans="12:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Z54">
+        <f t="shared" si="9"/>
+        <v>7.9003623188405789E-4</v>
+      </c>
+    </row>
+    <row r="55" spans="12:26" x14ac:dyDescent="0.55000000000000004">
       <c r="L55">
         <v>36.85</v>
       </c>
       <c r="M55">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.6500000000000021</v>
       </c>
       <c r="O55">
@@ -6451,13 +5534,17 @@
         <f t="shared" si="5"/>
         <v>6.4250000000000028E-3</v>
       </c>
-    </row>
-    <row r="56" spans="12:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Z55">
+        <f t="shared" si="9"/>
+        <v>7.6219715956558096E-4</v>
+      </c>
+    </row>
+    <row r="56" spans="12:26" x14ac:dyDescent="0.55000000000000004">
       <c r="L56">
         <v>43</v>
       </c>
       <c r="M56">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>6.1499999999999986</v>
       </c>
       <c r="O56">
@@ -6483,8 +5570,12 @@
         <f t="shared" si="5"/>
         <v>5.9249999999999988E-3</v>
       </c>
-    </row>
-    <row r="57" spans="12:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Z56">
+        <f t="shared" si="9"/>
+        <v>7.0650406504065033E-4</v>
+      </c>
+    </row>
+    <row r="57" spans="12:26" x14ac:dyDescent="0.55000000000000004">
       <c r="L57">
         <v>6.1</v>
       </c>
@@ -6515,8 +5606,12 @@
         <f t="shared" si="5"/>
         <v>5.875E-3</v>
       </c>
-    </row>
-    <row r="58" spans="12:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Z57">
+        <f t="shared" si="9"/>
+        <v>7.0093351548269585E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="12:26" x14ac:dyDescent="0.55000000000000004">
       <c r="L58">
         <v>12.05</v>
       </c>
@@ -6547,8 +5642,12 @@
         <f t="shared" si="5"/>
         <v>5.7250000000000018E-3</v>
       </c>
-    </row>
-    <row r="59" spans="12:25" x14ac:dyDescent="0.55000000000000004">
+      <c r="Z58">
+        <f t="shared" si="9"/>
+        <v>6.8422035480859031E-4</v>
+      </c>
+    </row>
+    <row r="59" spans="12:26" x14ac:dyDescent="0.55000000000000004">
       <c r="L59">
         <v>17.850000000000001</v>
       </c>
@@ -6579,362 +5678,12 @@
         <f t="shared" si="5"/>
         <v>5.575000000000001E-3</v>
       </c>
-    </row>
-    <row r="66" spans="10:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="L66" t="s">
-        <v>43</v>
-      </c>
-      <c r="M66" t="s">
-        <v>43</v>
-      </c>
-      <c r="N66" t="s">
-        <v>44</v>
-      </c>
-      <c r="O66" t="s">
-        <v>45</v>
-      </c>
-      <c r="R66" t="s">
-        <v>26</v>
-      </c>
-      <c r="S66" t="s">
-        <v>47</v>
-      </c>
-      <c r="V66" t="s">
-        <v>48</v>
-      </c>
-      <c r="X66" t="str">
-        <f t="shared" ref="X66:X74" si="10">R66</f>
-        <v>Time (s)</v>
-      </c>
-      <c r="Y66" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="67" spans="10:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="J67">
-        <v>0</v>
-      </c>
-      <c r="K67">
-        <v>10.15</v>
-      </c>
-      <c r="L67">
-        <f>K67</f>
-        <v>10.15</v>
-      </c>
-      <c r="M67">
-        <v>10.15</v>
-      </c>
-      <c r="N67">
-        <v>0.85</v>
-      </c>
-      <c r="O67">
-        <f>M67-$N$67/2</f>
-        <v>9.7249999999999996</v>
-      </c>
-      <c r="Q67">
-        <v>0.75</v>
-      </c>
-      <c r="R67">
-        <f>Q67*60</f>
-        <v>45</v>
-      </c>
-      <c r="S67">
-        <f>O67</f>
-        <v>9.7249999999999996</v>
-      </c>
-      <c r="V67">
-        <f>1/1000</f>
-        <v>1E-3</v>
-      </c>
-      <c r="X67">
-        <f t="shared" si="10"/>
-        <v>45</v>
-      </c>
-      <c r="Y67">
-        <f t="shared" ref="Y67:Y74" si="11">S67*$V$51</f>
-        <v>9.7249999999999993E-3</v>
-      </c>
-    </row>
-    <row r="68" spans="10:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="J68">
-        <v>3</v>
-      </c>
-      <c r="K68">
-        <v>18.649999999999999</v>
-      </c>
-      <c r="L68">
-        <f>K68-K67</f>
-        <v>8.4999999999999982</v>
-      </c>
-      <c r="M68">
-        <v>8.4999999999999982</v>
-      </c>
-      <c r="O68">
-        <f t="shared" ref="O68:O73" si="12">M68-$N$67/2</f>
-        <v>8.0749999999999975</v>
-      </c>
-      <c r="Q68">
-        <v>3</v>
-      </c>
-      <c r="R68">
-        <f t="shared" ref="R68:R74" si="13">Q68*60</f>
-        <v>180</v>
-      </c>
-      <c r="S68">
-        <f>O68</f>
-        <v>8.0749999999999975</v>
-      </c>
-      <c r="X68">
-        <f t="shared" si="10"/>
-        <v>180</v>
-      </c>
-      <c r="Y68">
-        <f t="shared" si="11"/>
-        <v>8.0749999999999971E-3</v>
-      </c>
-    </row>
-    <row r="69" spans="10:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="J69">
-        <v>6</v>
-      </c>
-      <c r="K69">
-        <v>7.2</v>
-      </c>
-      <c r="L69">
-        <f>K69</f>
-        <v>7.2</v>
-      </c>
-      <c r="M69">
-        <v>7.2</v>
-      </c>
-      <c r="O69">
-        <f t="shared" si="12"/>
-        <v>6.7750000000000004</v>
-      </c>
-      <c r="Q69">
-        <v>6</v>
-      </c>
-      <c r="R69">
-        <f t="shared" si="13"/>
-        <v>360</v>
-      </c>
-      <c r="S69">
-        <f t="shared" ref="S69:S74" si="14">O69</f>
-        <v>6.7750000000000004</v>
-      </c>
-      <c r="X69">
-        <f t="shared" si="10"/>
-        <v>360</v>
-      </c>
-      <c r="Y69">
-        <f t="shared" si="11"/>
-        <v>6.7750000000000006E-3</v>
-      </c>
-    </row>
-    <row r="70" spans="10:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="J70">
-        <v>10</v>
-      </c>
-      <c r="K70">
-        <v>12.65</v>
-      </c>
-      <c r="L70">
-        <f>K70-K69</f>
-        <v>5.45</v>
-      </c>
-      <c r="M70">
-        <v>5.45</v>
-      </c>
-      <c r="O70">
-        <f t="shared" si="12"/>
-        <v>5.0250000000000004</v>
-      </c>
-      <c r="Q70">
-        <v>10</v>
-      </c>
-      <c r="R70">
-        <f t="shared" si="13"/>
-        <v>600</v>
-      </c>
-      <c r="S70">
-        <f t="shared" si="14"/>
-        <v>5.0250000000000004</v>
-      </c>
-      <c r="X70">
-        <f t="shared" si="10"/>
-        <v>600</v>
-      </c>
-      <c r="Y70">
-        <f t="shared" si="11"/>
-        <v>5.0250000000000008E-3</v>
-      </c>
-      <c r="Z70" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="71" spans="10:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="J71">
-        <v>12</v>
-      </c>
-      <c r="K71">
-        <v>18.2</v>
-      </c>
-      <c r="L71">
-        <f>K71-K70</f>
-        <v>5.5499999999999989</v>
-      </c>
-      <c r="M71">
-        <v>5.5499999999999989</v>
-      </c>
-      <c r="O71">
-        <f t="shared" si="12"/>
-        <v>5.1249999999999991</v>
-      </c>
-      <c r="Q71">
-        <v>12</v>
-      </c>
-      <c r="R71">
-        <f t="shared" si="13"/>
-        <v>720</v>
-      </c>
-      <c r="S71">
-        <f t="shared" si="14"/>
-        <v>5.1249999999999991</v>
-      </c>
-      <c r="X71">
-        <f t="shared" si="10"/>
-        <v>720</v>
-      </c>
-      <c r="Y71">
-        <f t="shared" si="11"/>
-        <v>5.1249999999999993E-3</v>
-      </c>
-    </row>
-    <row r="72" spans="10:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="J72">
-        <v>15</v>
-      </c>
-      <c r="K72">
-        <v>23.75</v>
-      </c>
-      <c r="L72">
-        <f>K72-K71</f>
-        <v>5.5500000000000007</v>
-      </c>
-      <c r="M72">
-        <v>5.5500000000000007</v>
-      </c>
-      <c r="O72">
-        <f t="shared" si="12"/>
-        <v>5.1250000000000009</v>
-      </c>
-      <c r="Q72">
-        <v>15</v>
-      </c>
-      <c r="R72">
-        <f t="shared" si="13"/>
-        <v>900</v>
-      </c>
-      <c r="S72">
-        <f t="shared" si="14"/>
-        <v>5.1250000000000009</v>
-      </c>
-      <c r="X72">
-        <f t="shared" si="10"/>
-        <v>900</v>
-      </c>
-      <c r="Y72">
-        <f t="shared" si="11"/>
-        <v>5.1250000000000011E-3</v>
-      </c>
-    </row>
-    <row r="73" spans="10:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="J73" t="s">
-        <v>53</v>
-      </c>
-      <c r="K73">
-        <v>24.6</v>
-      </c>
-      <c r="L73">
-        <f>K73-K72</f>
-        <v>0.85000000000000142</v>
-      </c>
-      <c r="M73">
-        <v>5.1499999999999986</v>
-      </c>
-      <c r="O73">
-        <f t="shared" si="12"/>
-        <v>4.7249999999999988</v>
-      </c>
-      <c r="Q73">
-        <v>18</v>
-      </c>
-      <c r="R73">
-        <f t="shared" si="13"/>
-        <v>1080</v>
-      </c>
-      <c r="S73">
-        <f t="shared" si="14"/>
-        <v>4.7249999999999988</v>
-      </c>
-      <c r="X73">
-        <f t="shared" si="10"/>
-        <v>1080</v>
-      </c>
-      <c r="Y73">
-        <f t="shared" si="11"/>
-        <v>4.7249999999999992E-3</v>
-      </c>
-    </row>
-    <row r="74" spans="10:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="J74">
-        <v>18</v>
-      </c>
-      <c r="K74">
-        <v>29.75</v>
-      </c>
-      <c r="L74">
-        <f>K74-K73</f>
-        <v>5.1499999999999986</v>
-      </c>
-      <c r="M74">
-        <v>5.3500000000000014</v>
-      </c>
-      <c r="O74">
-        <f>M74-$N$67/2</f>
-        <v>4.9250000000000016</v>
-      </c>
-      <c r="Q74">
-        <v>21</v>
-      </c>
-      <c r="R74">
-        <f t="shared" si="13"/>
-        <v>1260</v>
-      </c>
-      <c r="S74">
-        <f t="shared" si="14"/>
-        <v>4.9250000000000016</v>
-      </c>
-      <c r="X74">
-        <f t="shared" si="10"/>
-        <v>1260</v>
-      </c>
-      <c r="Y74">
-        <f t="shared" si="11"/>
-        <v>4.9250000000000014E-3</v>
-      </c>
-    </row>
-    <row r="75" spans="10:26" x14ac:dyDescent="0.55000000000000004">
-      <c r="J75">
-        <v>21</v>
-      </c>
-      <c r="K75">
-        <v>35.1</v>
-      </c>
-      <c r="L75">
-        <f t="shared" ref="L75" si="15">K75-K74</f>
-        <v>5.3500000000000014</v>
-      </c>
+      <c r="Z59">
+        <f>Y59*((0.05/N$51) + (0.05/M59))</f>
+        <v>6.6750478927203084E-4</v>
+      </c>
+    </row>
+    <row r="75" spans="17:17" x14ac:dyDescent="0.55000000000000004">
       <c r="Q75" s="4"/>
     </row>
     <row r="82" spans="12:26" x14ac:dyDescent="0.55000000000000004">
@@ -6985,7 +5734,7 @@
         <v>60</v>
       </c>
       <c r="S83" s="4">
-        <f t="shared" ref="S83:S91" si="16">O83</f>
+        <f t="shared" ref="S83:S91" si="11">O83</f>
         <v>8.08</v>
       </c>
       <c r="V83">
@@ -7010,26 +5759,26 @@
         <v>8.0699999999999985</v>
       </c>
       <c r="O84" s="4">
-        <f t="shared" ref="O84:O91" si="17">M84-$N$83/2</f>
+        <f t="shared" ref="O84:O91" si="12">M84-$N$83/2</f>
         <v>7.8199999999999985</v>
       </c>
       <c r="Q84">
         <v>5</v>
       </c>
       <c r="R84">
-        <f t="shared" ref="R84:R90" si="18">Q84*60</f>
+        <f t="shared" ref="R84:R90" si="13">Q84*60</f>
         <v>300</v>
       </c>
       <c r="S84" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>7.8199999999999985</v>
       </c>
       <c r="X84">
-        <f t="shared" ref="X84:X91" si="19">R84</f>
+        <f t="shared" ref="X84:X91" si="14">R84</f>
         <v>300</v>
       </c>
       <c r="Y84">
-        <f t="shared" ref="Y84:Y91" si="20">S84*$V$51</f>
+        <f t="shared" ref="Y84:Y91" si="15">S84*$V$51</f>
         <v>7.8199999999999988E-3</v>
       </c>
     </row>
@@ -7041,7 +5790,7 @@
         <v>7.6</v>
       </c>
       <c r="O85" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v>7.35</v>
       </c>
       <c r="Q85">
@@ -7049,23 +5798,23 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="R85">
-        <f t="shared" si="18"/>
+        <f t="shared" si="13"/>
         <v>575</v>
       </c>
       <c r="S85" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>7.35</v>
       </c>
       <c r="X85">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>575</v>
       </c>
       <c r="Y85">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>7.3499999999999998E-3</v>
       </c>
       <c r="Z85" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="86" spans="12:26" x14ac:dyDescent="0.55000000000000004">
@@ -7077,26 +5826,26 @@
         <v>7.6</v>
       </c>
       <c r="O86" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v>7.35</v>
       </c>
       <c r="Q86">
         <v>13</v>
       </c>
       <c r="R86">
-        <f t="shared" si="18"/>
+        <f t="shared" si="13"/>
         <v>780</v>
       </c>
       <c r="S86" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>7.35</v>
       </c>
       <c r="X86">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>780</v>
       </c>
       <c r="Y86">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>7.3499999999999998E-3</v>
       </c>
     </row>
@@ -7109,26 +5858,26 @@
         <v>7</v>
       </c>
       <c r="O87" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v>6.75</v>
       </c>
       <c r="Q87">
         <v>17</v>
       </c>
       <c r="R87">
-        <f t="shared" si="18"/>
+        <f t="shared" si="13"/>
         <v>1020</v>
       </c>
       <c r="S87" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>6.75</v>
       </c>
       <c r="X87">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1020</v>
       </c>
       <c r="Y87">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>6.7499999999999999E-3</v>
       </c>
     </row>
@@ -7141,30 +5890,30 @@
         <v>7</v>
       </c>
       <c r="O88" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v>6.75</v>
       </c>
       <c r="Q88">
         <v>21</v>
       </c>
       <c r="R88">
-        <f t="shared" si="18"/>
+        <f t="shared" si="13"/>
         <v>1260</v>
       </c>
       <c r="S88" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>6.75</v>
       </c>
       <c r="X88">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1260</v>
       </c>
       <c r="Y88">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>6.7499999999999999E-3</v>
       </c>
       <c r="Z88" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="89" spans="12:26" x14ac:dyDescent="0.55000000000000004">
@@ -7176,26 +5925,26 @@
         <v>6.9000000000000021</v>
       </c>
       <c r="O89" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v>6.6500000000000021</v>
       </c>
       <c r="Q89">
         <v>25</v>
       </c>
       <c r="R89">
-        <f t="shared" si="18"/>
+        <f t="shared" si="13"/>
         <v>1500</v>
       </c>
       <c r="S89" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>6.6500000000000021</v>
       </c>
       <c r="X89">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1500</v>
       </c>
       <c r="Y89">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>6.6500000000000023E-3</v>
       </c>
     </row>
@@ -7207,7 +5956,7 @@
         <v>6.3</v>
       </c>
       <c r="O90" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v>6.05</v>
       </c>
       <c r="Q90">
@@ -7215,23 +5964,23 @@
         <v>29.333333333333332</v>
       </c>
       <c r="R90">
-        <f t="shared" si="18"/>
+        <f t="shared" si="13"/>
         <v>1760</v>
       </c>
       <c r="S90" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>6.05</v>
       </c>
       <c r="X90">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1760</v>
       </c>
       <c r="Y90">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>6.0499999999999998E-3</v>
       </c>
       <c r="Z90" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="91" spans="12:26" x14ac:dyDescent="0.55000000000000004">
@@ -7243,7 +5992,7 @@
         <v>6.45</v>
       </c>
       <c r="O91" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="12"/>
         <v>6.2</v>
       </c>
       <c r="Q91">
@@ -7254,21 +6003,21 @@
         <v>1980</v>
       </c>
       <c r="S91" s="4">
-        <f t="shared" si="16"/>
+        <f t="shared" si="11"/>
         <v>6.2</v>
       </c>
       <c r="X91">
-        <f t="shared" si="19"/>
+        <f t="shared" si="14"/>
         <v>1980</v>
       </c>
       <c r="Y91">
-        <f t="shared" si="20"/>
+        <f t="shared" si="15"/>
         <v>6.2000000000000006E-3</v>
       </c>
     </row>
     <row r="97" spans="12:30" x14ac:dyDescent="0.55000000000000004">
       <c r="AA97" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="AB97" s="6"/>
       <c r="AC97" s="6"/>
@@ -7305,7 +6054,7 @@
         <v>49</v>
       </c>
       <c r="AC98" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="99" spans="12:30" x14ac:dyDescent="0.55000000000000004">
@@ -7333,7 +6082,7 @@
         <v>81</v>
       </c>
       <c r="S99" s="4">
-        <f t="shared" ref="S99:S107" si="21">O99</f>
+        <f t="shared" ref="S99:S107" si="16">O99</f>
         <v>7.98</v>
       </c>
       <c r="V99">
@@ -7348,6 +6097,10 @@
         <f>S99*$V$51</f>
         <v>7.980000000000001E-3</v>
       </c>
+      <c r="Z99">
+        <f>Y99*((0.05/N$99) + (0.05/M99))</f>
+        <v>6.1789915966386621E-4</v>
+      </c>
       <c r="AA99">
         <v>81</v>
       </c>
@@ -7368,7 +6121,7 @@
         <v>7.1999999999999993</v>
       </c>
       <c r="O100" s="4">
-        <f t="shared" ref="O100:O110" si="22">M100-$N$99/2</f>
+        <f t="shared" ref="O100:O110" si="17">M100-$N$99/2</f>
         <v>6.85</v>
       </c>
       <c r="P100" s="4">
@@ -7382,16 +6135,20 @@
         <v>245</v>
       </c>
       <c r="S100" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>6.85</v>
       </c>
       <c r="X100">
-        <f t="shared" ref="X100:X107" si="23">R100</f>
+        <f t="shared" ref="X100:X107" si="18">R100</f>
         <v>245</v>
       </c>
       <c r="Y100">
-        <f t="shared" ref="Y100:Y107" si="24">S100*$V$51</f>
+        <f t="shared" ref="Y100:Y107" si="19">S100*$V$51</f>
         <v>6.8500000000000002E-3</v>
+      </c>
+      <c r="Z100">
+        <f t="shared" ref="Z100:Z110" si="20">Y100*((0.05/N$99) + (0.05/M100))</f>
+        <v>5.3685515873015926E-4</v>
       </c>
       <c r="AA100">
         <v>245</v>
@@ -7400,7 +6157,7 @@
         <v>6.5000000000000006E-3</v>
       </c>
       <c r="AC100" t="b">
-        <f t="shared" ref="AC100:AC110" si="25">AB100=Y100</f>
+        <f t="shared" ref="AC100:AC110" si="21">AB100=Y100</f>
         <v>0</v>
       </c>
     </row>
@@ -7412,7 +6169,7 @@
         <v>7.6</v>
       </c>
       <c r="O101" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>7.25</v>
       </c>
       <c r="P101" s="4"/>
@@ -7420,20 +6177,24 @@
         <v>7</v>
       </c>
       <c r="R101" s="4">
-        <f t="shared" ref="R101:R106" si="26">Q101*60</f>
+        <f t="shared" ref="R101:R106" si="22">Q101*60</f>
         <v>420</v>
       </c>
       <c r="S101" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>7.25</v>
       </c>
       <c r="X101">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>420</v>
       </c>
       <c r="Y101">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>7.2500000000000004E-3</v>
+      </c>
+      <c r="Z101">
+        <f t="shared" si="20"/>
+        <v>5.6555451127819612E-4</v>
       </c>
       <c r="AA101">
         <v>420</v>
@@ -7442,11 +6203,11 @@
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AC101" t="b">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AD101" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="102" spans="12:30" x14ac:dyDescent="0.55000000000000004">
@@ -7458,7 +6219,7 @@
         <v>5.7000000000000028</v>
       </c>
       <c r="O102" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>5.3500000000000032</v>
       </c>
       <c r="P102" s="4"/>
@@ -7466,20 +6227,24 @@
         <v>10</v>
       </c>
       <c r="R102" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>600</v>
       </c>
       <c r="S102" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>5.3500000000000032</v>
       </c>
       <c r="X102">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>600</v>
       </c>
       <c r="Y102">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>5.3500000000000032E-3</v>
+      </c>
+      <c r="Z102">
+        <f t="shared" si="20"/>
+        <v>4.2907268170426131E-4</v>
       </c>
       <c r="AA102">
         <v>600</v>
@@ -7488,11 +6253,11 @@
         <v>5.0000000000000036E-3</v>
       </c>
       <c r="AC102" t="b">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AD102" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="103" spans="12:30" x14ac:dyDescent="0.55000000000000004">
@@ -7504,7 +6269,7 @@
         <v>5.3999999999999986</v>
       </c>
       <c r="O103" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>5.0499999999999989</v>
       </c>
       <c r="P103" s="4"/>
@@ -7512,20 +6277,24 @@
         <v>13</v>
       </c>
       <c r="R103" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>780</v>
       </c>
       <c r="S103" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>5.0499999999999989</v>
       </c>
       <c r="X103">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>780</v>
       </c>
       <c r="Y103">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>5.0499999999999989E-3</v>
+      </c>
+      <c r="Z103">
+        <f t="shared" si="20"/>
+        <v>4.0747354497354529E-4</v>
       </c>
       <c r="AA103">
         <v>780</v>
@@ -7534,11 +6303,11 @@
         <v>4.6999999999999993E-3</v>
       </c>
       <c r="AC103" t="b">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AD103" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="104" spans="12:30" x14ac:dyDescent="0.55000000000000004">
@@ -7550,7 +6319,7 @@
         <v>5.1000000000000014</v>
       </c>
       <c r="O104" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>4.7500000000000018</v>
       </c>
       <c r="P104" s="4"/>
@@ -7562,16 +6331,20 @@
         <v>960</v>
       </c>
       <c r="S104" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>4.7500000000000018</v>
       </c>
       <c r="X104">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>960</v>
       </c>
       <c r="Y104">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>4.7500000000000016E-3</v>
+      </c>
+      <c r="Z104">
+        <f t="shared" si="20"/>
+        <v>3.8585434173669513E-4</v>
       </c>
       <c r="AA104">
         <v>960</v>
@@ -7580,7 +6353,7 @@
         <v>4.400000000000002E-3</v>
       </c>
       <c r="AC104" t="b">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7593,7 +6366,7 @@
         <v>4.8999999999999986</v>
       </c>
       <c r="O105" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>4.5499999999999989</v>
       </c>
       <c r="P105" s="4"/>
@@ -7601,20 +6374,24 @@
         <v>19</v>
       </c>
       <c r="R105" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1140</v>
       </c>
       <c r="S105" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>4.5499999999999989</v>
       </c>
       <c r="X105">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>1140</v>
       </c>
       <c r="Y105">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>4.5499999999999994E-3</v>
+      </c>
+      <c r="Z105">
+        <f t="shared" si="20"/>
+        <v>3.7142857142857181E-4</v>
       </c>
       <c r="AA105">
         <v>1140</v>
@@ -7623,11 +6400,11 @@
         <v>4.15E-3</v>
       </c>
       <c r="AC105" t="b">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AD105" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="106" spans="12:30" x14ac:dyDescent="0.55000000000000004">
@@ -7639,7 +6416,7 @@
         <v>4.5</v>
       </c>
       <c r="O106" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>4.1500000000000004</v>
       </c>
       <c r="P106" s="4"/>
@@ -7647,20 +6424,24 @@
         <v>22</v>
       </c>
       <c r="R106" s="4">
-        <f t="shared" si="26"/>
+        <f t="shared" si="22"/>
         <v>1320</v>
       </c>
       <c r="S106" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>4.1500000000000004</v>
       </c>
       <c r="X106">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>1320</v>
       </c>
       <c r="Y106">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>4.15E-3</v>
+      </c>
+      <c r="Z106">
+        <f t="shared" si="20"/>
+        <v>3.4253968253968286E-4</v>
       </c>
       <c r="AA106">
         <v>1320</v>
@@ -7669,7 +6450,7 @@
         <v>3.8E-3</v>
       </c>
       <c r="AC106" t="b">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7682,7 +6463,7 @@
         <v>4.3000000000000007</v>
       </c>
       <c r="O107" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>3.9500000000000011</v>
       </c>
       <c r="P107" s="4"/>
@@ -7694,16 +6475,20 @@
         <v>1500</v>
       </c>
       <c r="S107" s="4">
-        <f t="shared" si="21"/>
+        <f t="shared" si="16"/>
         <v>3.9500000000000011</v>
       </c>
       <c r="X107">
-        <f t="shared" si="23"/>
+        <f t="shared" si="18"/>
         <v>1500</v>
       </c>
       <c r="Y107">
-        <f t="shared" si="24"/>
+        <f t="shared" si="19"/>
         <v>3.9500000000000013E-3</v>
+      </c>
+      <c r="Z107">
+        <f t="shared" si="20"/>
+        <v>3.2807308970099708E-4</v>
       </c>
       <c r="AA107">
         <v>1500</v>
@@ -7712,7 +6497,7 @@
         <v>3.6000000000000016E-3</v>
       </c>
       <c r="AC107" t="b">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="AD107" t="s">
@@ -7728,7 +6513,7 @@
         <v>4.0299999999999994</v>
       </c>
       <c r="O108" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>3.6799999999999997</v>
       </c>
       <c r="P108" s="4"/>
@@ -7736,20 +6521,24 @@
         <v>28</v>
       </c>
       <c r="R108" s="4">
-        <f t="shared" ref="R108:R109" si="27">Q108*60</f>
+        <f t="shared" ref="R108:R109" si="23">Q108*60</f>
         <v>1680</v>
       </c>
       <c r="S108" s="4">
-        <f t="shared" ref="S108:S110" si="28">O108</f>
+        <f t="shared" ref="S108:S110" si="24">O108</f>
         <v>3.6799999999999997</v>
       </c>
       <c r="X108">
-        <f t="shared" ref="X108:X110" si="29">R108</f>
+        <f t="shared" ref="X108:X110" si="25">R108</f>
         <v>1680</v>
       </c>
       <c r="Y108">
-        <f t="shared" ref="Y108:Y110" si="30">S108*$V$51</f>
+        <f t="shared" ref="Y108:Y110" si="26">S108*$V$51</f>
         <v>3.6799999999999997E-3</v>
+      </c>
+      <c r="Z108">
+        <f t="shared" si="20"/>
+        <v>3.0851471109535656E-4</v>
       </c>
       <c r="AA108">
         <v>1680</v>
@@ -7758,7 +6547,7 @@
         <v>3.3300000000000001E-3</v>
       </c>
       <c r="AC108" t="b">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7771,7 +6560,7 @@
         <v>4.0699999999999985</v>
       </c>
       <c r="O109" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>3.7199999999999989</v>
       </c>
       <c r="P109" s="4"/>
@@ -7779,20 +6568,24 @@
         <v>31</v>
       </c>
       <c r="R109" s="4">
-        <f t="shared" si="27"/>
+        <f t="shared" si="23"/>
         <v>1860</v>
       </c>
       <c r="S109" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="24"/>
         <v>3.7199999999999989</v>
       </c>
       <c r="X109">
-        <f t="shared" si="29"/>
+        <f t="shared" si="25"/>
         <v>1860</v>
       </c>
       <c r="Y109">
-        <f t="shared" si="30"/>
+        <f t="shared" si="26"/>
         <v>3.7199999999999989E-3</v>
+      </c>
+      <c r="Z109">
+        <f t="shared" si="20"/>
+        <v>3.1141453141453161E-4</v>
       </c>
       <c r="AA109">
         <v>1860</v>
@@ -7801,7 +6594,7 @@
         <v>3.2499999999999999E-3</v>
       </c>
       <c r="AC109" t="b">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>
@@ -7814,7 +6607,7 @@
         <v>3.9000000000000021</v>
       </c>
       <c r="O110" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="17"/>
         <v>3.5500000000000025</v>
       </c>
       <c r="P110" s="4"/>
@@ -7826,16 +6619,20 @@
         <v>2040</v>
       </c>
       <c r="S110" s="4">
-        <f t="shared" si="28"/>
+        <f t="shared" si="24"/>
         <v>3.5500000000000025</v>
       </c>
       <c r="X110">
-        <f t="shared" si="29"/>
+        <f t="shared" si="25"/>
         <v>2040</v>
       </c>
       <c r="Y110">
-        <f t="shared" si="30"/>
+        <f t="shared" si="26"/>
         <v>3.5500000000000024E-3</v>
+      </c>
+      <c r="Z110">
+        <f t="shared" si="20"/>
+        <v>2.9908424908424956E-4</v>
       </c>
       <c r="AA110">
         <v>2040</v>
@@ -7844,7 +6641,7 @@
         <v>3.2000000000000028E-3</v>
       </c>
       <c r="AC110" t="b">
-        <f t="shared" si="25"/>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
So close to being done my Chemistry IA. I fixed the parameter estimation script to actually take in the temperature vector. Comparing the simulated to the experimental concentration profiles is extremely promising.
</commit_message>
<xml_diff>
--- a/Excel Projects/Esterification Lab Data Logging.xlsx
+++ b/Excel Projects/Esterification Lab Data Logging.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wille\Desktop\Legacy-Projects-And-Code-Will-Martin\Excel Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wille\Desktop\Projects-And-Code-Will-Martin\Excel Projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB920CF-1AC7-4612-836A-F5AD6BA44E90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3E8B1B-09DF-4E7C-B05A-2C2E64F12D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{27043B7B-2271-401B-B46D-49CA3CF67942}"/>
+    <workbookView xWindow="4686" yWindow="2550" windowWidth="17280" windowHeight="8994" xr2:uid="{27043B7B-2271-401B-B46D-49CA3CF67942}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -255,8 +255,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -287,7 +288,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -305,6 +306,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1489,13 +1491,13 @@
             <c:numRef>
               <c:f>Sheet1!$AB$99:$AB$110</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.00000</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>7.6300000000000014E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.5000000000000006E-3</c:v>
+                  <c:v>6.4999999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.4999999999999997E-3</c:v>
@@ -1631,7 +1633,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -4409,8 +4411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16E9B97C-057F-4C1E-9083-78A721E3BFF1}">
   <dimension ref="B3:AD110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K47" workbookViewId="0">
-      <selection activeCell="Z51" sqref="Z51:Z59"/>
+    <sheetView tabSelected="1" topLeftCell="X96" workbookViewId="0">
+      <selection activeCell="AC98" sqref="AC98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6104,7 +6106,7 @@
       <c r="AA99">
         <v>81</v>
       </c>
-      <c r="AB99">
+      <c r="AB99" s="9">
         <v>7.6300000000000014E-3</v>
       </c>
       <c r="AC99" t="b">
@@ -6147,17 +6149,17 @@
         <v>6.8500000000000002E-3</v>
       </c>
       <c r="Z100">
-        <f t="shared" ref="Z100:Z110" si="20">Y100*((0.05/N$99) + (0.05/M100))</f>
+        <f>Y100*((0.05/N$99) + (0.05/M100))</f>
         <v>5.3685515873015926E-4</v>
       </c>
       <c r="AA100">
         <v>245</v>
       </c>
-      <c r="AB100">
-        <v>6.5000000000000006E-3</v>
+      <c r="AB100" s="9">
+        <v>6.4999999999999997E-3</v>
       </c>
       <c r="AC100" t="b">
-        <f t="shared" ref="AC100:AC110" si="21">AB100=Y100</f>
+        <f>AB100=Y100</f>
         <v>0</v>
       </c>
     </row>
@@ -6177,7 +6179,7 @@
         <v>7</v>
       </c>
       <c r="R101" s="4">
-        <f t="shared" ref="R101:R106" si="22">Q101*60</f>
+        <f t="shared" ref="R101:R106" si="20">Q101*60</f>
         <v>420</v>
       </c>
       <c r="S101" s="4">
@@ -6193,17 +6195,17 @@
         <v>7.2500000000000004E-3</v>
       </c>
       <c r="Z101">
-        <f t="shared" si="20"/>
+        <f t="shared" ref="Z100:Z110" si="21">Y101*((0.05/N$99) + (0.05/M101))</f>
         <v>5.6555451127819612E-4</v>
       </c>
       <c r="AA101">
         <v>420</v>
       </c>
-      <c r="AB101">
+      <c r="AB101" s="9">
         <v>5.4999999999999997E-3</v>
       </c>
       <c r="AC101" t="b">
-        <f t="shared" si="21"/>
+        <f>AB101=Y101</f>
         <v>0</v>
       </c>
       <c r="AD101" t="s">
@@ -6227,7 +6229,7 @@
         <v>10</v>
       </c>
       <c r="R102" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>600</v>
       </c>
       <c r="S102" s="4">
@@ -6243,17 +6245,17 @@
         <v>5.3500000000000032E-3</v>
       </c>
       <c r="Z102">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>4.2907268170426131E-4</v>
       </c>
       <c r="AA102">
         <v>600</v>
       </c>
-      <c r="AB102">
+      <c r="AB102" s="9">
         <v>5.0000000000000036E-3</v>
       </c>
       <c r="AC102" t="b">
-        <f t="shared" si="21"/>
+        <f t="shared" ref="AC100:AC110" si="22">AB102=Y102</f>
         <v>0</v>
       </c>
       <c r="AD102" t="s">
@@ -6277,7 +6279,7 @@
         <v>13</v>
       </c>
       <c r="R103" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>780</v>
       </c>
       <c r="S103" s="4">
@@ -6293,17 +6295,17 @@
         <v>5.0499999999999989E-3</v>
       </c>
       <c r="Z103">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>4.0747354497354529E-4</v>
       </c>
       <c r="AA103">
         <v>780</v>
       </c>
-      <c r="AB103">
+      <c r="AB103" s="9">
         <v>4.6999999999999993E-3</v>
       </c>
       <c r="AC103" t="b">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AD103" t="s">
@@ -6343,17 +6345,17 @@
         <v>4.7500000000000016E-3</v>
       </c>
       <c r="Z104">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3.8585434173669513E-4</v>
       </c>
       <c r="AA104">
         <v>960</v>
       </c>
-      <c r="AB104">
+      <c r="AB104" s="9">
         <v>4.400000000000002E-3</v>
       </c>
       <c r="AC104" t="b">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -6374,7 +6376,7 @@
         <v>19</v>
       </c>
       <c r="R105" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>1140</v>
       </c>
       <c r="S105" s="4">
@@ -6390,17 +6392,17 @@
         <v>4.5499999999999994E-3</v>
       </c>
       <c r="Z105">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3.7142857142857181E-4</v>
       </c>
       <c r="AA105">
         <v>1140</v>
       </c>
-      <c r="AB105">
+      <c r="AB105" s="9">
         <v>4.15E-3</v>
       </c>
       <c r="AC105" t="b">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AD105" t="s">
@@ -6424,7 +6426,7 @@
         <v>22</v>
       </c>
       <c r="R106" s="4">
-        <f t="shared" si="22"/>
+        <f t="shared" si="20"/>
         <v>1320</v>
       </c>
       <c r="S106" s="4">
@@ -6440,17 +6442,17 @@
         <v>4.15E-3</v>
       </c>
       <c r="Z106">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3.4253968253968286E-4</v>
       </c>
       <c r="AA106">
         <v>1320</v>
       </c>
-      <c r="AB106">
+      <c r="AB106" s="9">
         <v>3.8E-3</v>
       </c>
       <c r="AC106" t="b">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -6487,17 +6489,17 @@
         <v>3.9500000000000013E-3</v>
       </c>
       <c r="Z107">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3.2807308970099708E-4</v>
       </c>
       <c r="AA107">
         <v>1500</v>
       </c>
-      <c r="AB107">
+      <c r="AB107" s="9">
         <v>3.6000000000000016E-3</v>
       </c>
       <c r="AC107" t="b">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="AD107" t="s">
@@ -6537,17 +6539,17 @@
         <v>3.6799999999999997E-3</v>
       </c>
       <c r="Z108">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3.0851471109535656E-4</v>
       </c>
       <c r="AA108">
         <v>1680</v>
       </c>
-      <c r="AB108">
+      <c r="AB108" s="9">
         <v>3.3300000000000001E-3</v>
       </c>
       <c r="AC108" t="b">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -6584,17 +6586,17 @@
         <v>3.7199999999999989E-3</v>
       </c>
       <c r="Z109">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>3.1141453141453161E-4</v>
       </c>
       <c r="AA109">
         <v>1860</v>
       </c>
-      <c r="AB109">
+      <c r="AB109" s="9">
         <v>3.2499999999999999E-3</v>
       </c>
       <c r="AC109" t="b">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>
@@ -6631,17 +6633,17 @@
         <v>3.5500000000000024E-3</v>
       </c>
       <c r="Z110">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>2.9908424908424956E-4</v>
       </c>
       <c r="AA110">
         <v>2040</v>
       </c>
-      <c r="AB110">
+      <c r="AB110" s="9">
         <v>3.2000000000000028E-3</v>
       </c>
       <c r="AC110" t="b">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>